<commit_message>
Added Custom 404 pages and some functional part
</commit_message>
<xml_diff>
--- a/smartexcel/PDF-Files/Combined-Data-Sheet.xlsx
+++ b/smartexcel/PDF-Files/Combined-Data-Sheet.xlsx
@@ -493,92 +493,160 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>form_17.pdf</t>
+          <t>form_23.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Volume 2</t>
+          <t>Volume 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>Knowledge of pharmaceutical equipments, Medicine effects, Behavior, Functionality, etc.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>Double-check where the date string is coming from. Ensure that any JavaScript or frontend frameworks formatting dates are consistent where the date string is coming from. Ensure that any JavaScript or frontend frameworks formatting dates are consistent</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>Observation of bioplant on the presence of WHO.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>emit a second event from the view. In the previous article, we used the HX-Trigger header to raise a JavaScript event from the Django</t>
-        </is>
-      </c>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>form_16.pdf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+          <t>form_23.pdf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Volume 1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Knowledge of pharmaceutical equipments, Medicine effects, Behavior, Functionality, etc.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Double-check where the date string is coming from. Ensure that any JavaScript or frontend frameworks formatting dates are consistent where the date string is coming from. Ensure that any JavaScript or frontend frameworks formatting dates are consistent</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Observation of bioplant on the presence of WHO.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>form_16.pdf</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+          <t>form_23.pdf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Volume 1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Knowledge of pharmaceutical equipments, Medicine effects, Behavior, Functionality, etc.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Double-check where the date string is coming from. Ensure that any JavaScript or frontend frameworks formatting dates are consistent where the date string is coming from. Ensure that any JavaScript or frontend frameworks formatting dates are consistent</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Observation of bioplant on the presence of WHO.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>It looks like your message just says "text". Did you have a specific question or topic you'd like to discuss regarding text or anything else? Feel free to let me know how I can assist you!It looks like your message just says "text". Did you have a specifi</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>